<commit_message>
Tank City  by scratch _20200415
</commit_message>
<xml_diff>
--- a/Tank City  by scratch _20200415/NOTE.xlsx
+++ b/Tank City  by scratch _20200415/NOTE.xlsx
@@ -28,9 +28,6 @@
     <t>可以重新开始-ok</t>
   </si>
   <si>
-    <t>角色可以出现移动-敌我双方开始登场-ok</t>
-  </si>
-  <si>
     <t>角色可以移动-我方可以移动-ok</t>
   </si>
   <si>
@@ -49,13 +46,20 @@
     <t>敌人1-2-3发射子弹-敌方1-2-3发射子弹-ok</t>
   </si>
   <si>
-    <t>剩下：子弹积木与背景积木，全部角色默认属性，全部参数默认值，</t>
-  </si>
-  <si>
-    <t xml:space="preserve">晚上：步数？ XY坐标？造型-声音-变量-代码-广播 </t>
-  </si>
-  <si>
-    <t>我方移动yTemp_编程总动员32？？？</t>
+    <t>角色可以出现移动-背景搭建完成-ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剩下：全部角色默认属性，全部参数默认值，子弹积木与背景积木-ok，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我方移动yTemp_编程总动员32？？？-ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">晚上：步数？-ok XY坐标？-ok 造型-声音-变量-代码-广播-ok </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -401,7 +405,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
@@ -415,7 +421,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
@@ -429,7 +437,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
@@ -444,7 +454,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -475,58 +485,58 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:8">

</xml_diff>